<commit_message>
fix data test Login
</commit_message>
<xml_diff>
--- a/TestResults.xlsx
+++ b/TestResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>Username</t>
   </si>
@@ -44,19 +44,19 @@
     <t>mnp456hashed</t>
   </si>
   <si>
+    <t>jane@example.com</t>
+  </si>
+  <si>
+    <t>xyz987hashed</t>
+  </si>
+  <si>
     <t>invalidUser</t>
   </si>
   <si>
     <t>Fail</t>
   </si>
   <si>
-    <t>validUser</t>
-  </si>
-  <si>
     <t>invalidPass</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -101,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -160,10 +160,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>7</v>
@@ -177,69 +177,35 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>6</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s" s="0">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
retry to run testng
</commit_message>
<xml_diff>
--- a/TestResults.xlsx
+++ b/TestResults.xlsx
@@ -38,6 +38,9 @@
     <t>Pass</t>
   </si>
   <si>
+    <t>Fail</t>
+  </si>
+  <si>
     <t>michael@example.com</t>
   </si>
   <si>
@@ -51,9 +54,6 @@
   </si>
   <si>
     <t>invalidUser</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
   <si>
     <t>invalidPass</t>
@@ -135,58 +135,58 @@
         <v>7</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>7</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>7</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>6</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>7</v>
@@ -200,10 +200,10 @@
         <v>14</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>7</v>

</xml_diff>